<commit_message>
previously downloaded excel files changed?
</commit_message>
<xml_diff>
--- a/nlp/data/VCHAINS/4296954028_VCHAINS.xlsx
+++ b/nlp/data/VCHAINS/4296954028_VCHAINS.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <x:si>
     <x:t>Value Chains</x:t>
   </x:si>
@@ -31,7 +31,7 @@
     <x:t>Company Name</x:t>
   </x:si>
   <x:si>
-    <x:t>Lite-On Technology Corp</x:t>
+    <x:t>Japan Display Inc</x:t>
   </x:si>
   <x:si>
     <x:t>Company Id</x:t>
@@ -94,37 +94,49 @@
     <x:t>A</x:t>
   </x:si>
   <x:si>
-    <x:t>Roku Inc</x:t>
+    <x:t>LG Display Co Ltd</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Korea; Republic (S. Korea)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Electronic Equipment &amp; Parts</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BB</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TPK Holding Co Ltd</x:t>
   </x:si>
   <x:si>
     <x:t>Supplier</x:t>
   </x:si>
   <x:si>
-    <x:t>Entertainment Production</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Cypress Semiconductor Corp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Private</x:t>
+    <x:t>Taiwan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>A-</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IQE PLC</x:t>
+  </x:si>
+  <x:si>
+    <x:t>United Kingdom</x:t>
   </x:si>
   <x:si>
     <x:t>Semiconductors</x:t>
   </x:si>
   <x:si>
-    <x:t>BBB-</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Optomec Inc</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Electronic Equipment &amp; Parts</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Kioxia Holdings Corp</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Japan</x:t>
+    <x:t>BB-</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lumentum Holdings Inc</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Communications &amp; Networking</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BBB+</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -585,17 +597,17 @@
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="15.700625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="26.300625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="7.830625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="22.640625" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="6.050625" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="12.710625" style="0" customWidth="1"/>
     <x:col min="5" max="5" width="23.040625" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="26.790625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="28.520625" style="0" customWidth="1"/>
     <x:col min="7" max="7" width="20.190625" style="0" customWidth="1"/>
     <x:col min="8" max="8" width="16.840625000000003" style="0" customWidth="1"/>
     <x:col min="9" max="9" width="21.920625" style="0" customWidth="1"/>
     <x:col min="10" max="10" width="10.410625" style="0" customWidth="1"/>
     <x:col min="11" max="11" width="14.180625000000001" style="0" customWidth="1"/>
-    <x:col min="12" max="12" width="14.880625" style="0" customWidth="1"/>
+    <x:col min="12" max="12" width="18.300625" style="0" customWidth="1"/>
     <x:col min="13" max="13" width="9.570625" style="0" customWidth="1"/>
     <x:col min="14" max="14" width="14.480625" style="0" customWidth="1"/>
   </x:cols>
@@ -605,7 +617,7 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="B1" s="2">
-        <x:v>44595.9256944444</x:v>
+        <x:v>44597.8576388889</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:14" customFormat="1" ht="32.26" customHeight="1">
@@ -639,7 +651,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="B4" s="5" t="n">
-        <x:v>4295891508</x:v>
+        <x:v>4296954028</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:14">
@@ -709,16 +721,16 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="H7" s="8">
-        <x:v>43132</x:v>
+        <x:v>44028</x:v>
       </x:c>
       <x:c r="I7" s="9" t="n">
-        <x:v>1463</x:v>
+        <x:v>569</x:v>
       </x:c>
       <x:c r="J7" s="5" t="n">
-        <x:v>2</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="K7" s="5" t="n">
-        <x:v>1</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="L7" s="5" t="n">
         <x:v>365817000000</x:v>
@@ -732,7 +744,7 @@
     </x:row>
     <x:row r="8" spans="1:14">
       <x:c r="A8" s="5" t="n">
-        <x:v>4297900917</x:v>
+        <x:v>4295882602</x:v>
       </x:c>
       <x:c r="B8" s="5" t="s">
         <x:v>23</x:v>
@@ -741,158 +753,170 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="D8" s="5" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="E8" s="5" t="s">
         <x:v>24</x:v>
-      </x:c>
-      <x:c r="E8" s="5" t="s">
-        <x:v>20</x:v>
       </x:c>
       <x:c r="F8" s="5" t="s">
         <x:v>25</x:v>
       </x:c>
       <x:c r="G8" s="7" t="n">
-        <x:v>0.55678434528</x:v>
+        <x:v>0.30295536</x:v>
       </x:c>
       <x:c r="H8" s="8">
-        <x:v>43062</x:v>
+        <x:v>43487</x:v>
       </x:c>
       <x:c r="I8" s="9" t="n">
-        <x:v>1533</x:v>
+        <x:v>1110</x:v>
       </x:c>
       <x:c r="J8" s="5" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="K8" s="5" t="n">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="K8" s="5" t="n">
-        <x:v>3</x:v>
-      </x:c>
       <x:c r="L8" s="5" t="n">
-        <x:v>1778388000</x:v>
+        <x:v>26127175997.2868</x:v>
       </x:c>
       <x:c r="M8" s="5" t="n">
-        <x:v>93</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="N8" s="5" t="s">
-        <x:v>22</x:v>
+        <x:v>26</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:14">
       <x:c r="A9" s="5" t="n">
-        <x:v>4295903116</x:v>
+        <x:v>4297787586</x:v>
       </x:c>
       <x:c r="B9" s="5" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="C9" s="5" t="s">
-        <x:v>27</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D9" s="5" t="s">
-        <x:v>24</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="E9" s="5" t="s">
-        <x:v>20</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="F9" s="5" t="s">
-        <x:v>28</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="G9" s="7" t="n">
-        <x:v>0.30366456</x:v>
+        <x:v>0.301104</x:v>
       </x:c>
       <x:c r="H9" s="8">
-        <x:v>41156</x:v>
+        <x:v>43658</x:v>
       </x:c>
       <x:c r="I9" s="9" t="n">
-        <x:v>3439</x:v>
+        <x:v>939</x:v>
       </x:c>
       <x:c r="J9" s="5" t="n">
-        <x:v>1</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="K9" s="5" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="L9" s="5" t="n">
-        <x:v>2205314000</x:v>
-      </x:c>
-      <x:c r="M9" s="5" t="s"/>
+        <x:v>3893466268.34875</x:v>
+      </x:c>
+      <x:c r="M9" s="5" t="n">
+        <x:v>41</x:v>
+      </x:c>
       <x:c r="N9" s="5" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:14">
       <x:c r="A10" s="5" t="n">
-        <x:v>4297422171</x:v>
+        <x:v>4295896478</x:v>
       </x:c>
       <x:c r="B10" s="5" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C10" s="5" t="s">
-        <x:v>27</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D10" s="5" t="s">
-        <x:v>24</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="E10" s="5" t="s">
-        <x:v>20</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="F10" s="5" t="s">
-        <x:v>31</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="G10" s="7" t="n">
-        <x:v>0.29733864</x:v>
+        <x:v>0.28509432</x:v>
       </x:c>
       <x:c r="H10" s="8">
-        <x:v>42452</x:v>
+        <x:v>43418</x:v>
       </x:c>
       <x:c r="I10" s="9" t="n">
-        <x:v>2143</x:v>
+        <x:v>1179</x:v>
       </x:c>
       <x:c r="J10" s="5" t="n">
-        <x:v>1</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="K10" s="5" t="n">
         <x:v>2</x:v>
       </x:c>
       <x:c r="L10" s="5" t="n">
-        <x:v>8007154</x:v>
-      </x:c>
-      <x:c r="M10" s="5" t="s"/>
-      <x:c r="N10" s="5" t="s"/>
+        <x:v>228475432.879399</x:v>
+      </x:c>
+      <x:c r="M10" s="5" t="n">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="N10" s="5" t="s">
+        <x:v>34</x:v>
+      </x:c>
     </x:row>
     <x:row r="11" spans="1:14">
       <x:c r="A11" s="5" t="n">
-        <x:v>5068663189</x:v>
+        <x:v>5045880046</x:v>
       </x:c>
       <x:c r="B11" s="5" t="s">
-        <x:v>32</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="C11" s="5" t="s">
-        <x:v>27</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="D11" s="5" t="s">
         <x:v>19</x:v>
       </x:c>
       <x:c r="E11" s="5" t="s">
-        <x:v>33</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="F11" s="5" t="s">
-        <x:v>28</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="G11" s="7" t="n">
-        <x:v>0.2897888</x:v>
+        <x:v>0.28391264</x:v>
       </x:c>
       <x:c r="H11" s="8">
-        <x:v>43710</x:v>
+        <x:v>43418</x:v>
       </x:c>
       <x:c r="I11" s="9" t="n">
-        <x:v>885</x:v>
+        <x:v>1179</x:v>
       </x:c>
       <x:c r="J11" s="5" t="n">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="K11" s="5" t="n">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="L11" s="5" t="s"/>
-      <x:c r="M11" s="5" t="s"/>
-      <x:c r="N11" s="5" t="s"/>
+      <x:c r="L11" s="5" t="n">
+        <x:v>1742800000</x:v>
+      </x:c>
+      <x:c r="M11" s="5" t="n">
+        <x:v>91</x:v>
+      </x:c>
+      <x:c r="N11" s="5" t="s">
+        <x:v>37</x:v>
+      </x:c>
     </x:row>
   </x:sheetData>
   <x:mergeCells count="1">

</xml_diff>